<commit_message>
Pushing com port project folder
</commit_message>
<xml_diff>
--- a/Schedule Template.xlsx
+++ b/Schedule Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stuconestogacon-my.sharepoint.com/personal/jrussell2240_conestogac_on_ca/Documents/Conestoga/Year2/sem1/Projects/CMS/CMS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachm\OneDrive\Desktop\Sem 1\Eng. Projects\CMS\Source Code\CMS\CMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{6B85AC7F-8B9F-461C-8C99-F3F76250EC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD59ABB4-7D3E-4497-BD0D-E30AFCF8921A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87302B7A-1001-4404-BE6A-21ABB79B4BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1093,6 +1093,33 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1117,37 +1144,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1432,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,26 +1445,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
       <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63"/>
-      <c r="B2" s="61"/>
+      <c r="A2" s="72"/>
+      <c r="B2" s="70"/>
       <c r="C2" s="57">
         <v>1</v>
       </c>
@@ -1489,7 +1489,7 @@
       <c r="J2" s="56"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68">
+      <c r="A3" s="63">
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -1505,11 +1505,11 @@
       <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="69"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="75" t="s">
         <v>70</v>
       </c>
       <c r="D4" s="2"/>
@@ -1521,11 +1521,11 @@
       <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="69"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="67"/>
+      <c r="C5" s="76"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1535,7 +1535,7 @@
       <c r="J5" s="32"/>
     </row>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="69"/>
+      <c r="A6" s="64"/>
       <c r="B6" s="17" t="s">
         <v>5</v>
       </c>
@@ -1549,7 +1549,7 @@
       <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="69"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="16" t="s">
         <v>6</v>
       </c>
@@ -1565,14 +1565,14 @@
       <c r="J7" s="32"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="69"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="71" t="s">
+      <c r="C8" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="72"/>
+      <c r="D8" s="78"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1581,7 +1581,7 @@
       <c r="J8" s="32"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="69"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="17" t="s">
         <v>7</v>
       </c>
@@ -1595,7 +1595,7 @@
       <c r="J9" s="32"/>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="69"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="18" t="s">
         <v>8</v>
       </c>
@@ -1611,7 +1611,7 @@
       <c r="J10" s="32"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="69"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="16" t="s">
         <v>9</v>
       </c>
@@ -1627,7 +1627,7 @@
       <c r="J11" s="32"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="69"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="17" t="s">
         <v>10</v>
       </c>
@@ -1641,7 +1641,7 @@
       <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="69"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="16" t="s">
         <v>11</v>
       </c>
@@ -1657,7 +1657,7 @@
       <c r="J13" s="32"/>
     </row>
     <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="69"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="17" t="s">
         <v>13</v>
       </c>
@@ -1673,7 +1673,7 @@
       <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="70"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="19" t="s">
         <v>15</v>
       </c>
@@ -1689,7 +1689,7 @@
       <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68">
+      <c r="A16" s="63">
         <v>2</v>
       </c>
       <c r="B16" s="15" t="s">
@@ -1705,12 +1705,12 @@
       <c r="J16" s="32"/>
     </row>
     <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="69"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="28"/>
-      <c r="D17" s="73" t="s">
+      <c r="D17" s="66" t="s">
         <v>70</v>
       </c>
       <c r="E17" s="3"/>
@@ -1721,12 +1721,12 @@
       <c r="J17" s="32"/>
     </row>
     <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="69"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="28"/>
-      <c r="D18" s="74"/>
+      <c r="D18" s="68"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1735,12 +1735,12 @@
       <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="69"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="28"/>
-      <c r="D19" s="75"/>
+      <c r="D19" s="67"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1749,7 +1749,7 @@
       <c r="J19" s="32"/>
     </row>
     <row r="20" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="69"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="17" t="s">
         <v>19</v>
       </c>
@@ -1763,7 +1763,7 @@
       <c r="J20" s="32"/>
     </row>
     <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="69"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="16" t="s">
         <v>20</v>
       </c>
@@ -1779,7 +1779,7 @@
       <c r="J21" s="32"/>
     </row>
     <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="69"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="17" t="s">
         <v>21</v>
       </c>
@@ -1794,12 +1794,12 @@
       <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" ht="33.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="69"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="20" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="28"/>
-      <c r="D23" s="73" t="s">
+      <c r="D23" s="66" t="s">
         <v>74</v>
       </c>
       <c r="E23" s="3"/>
@@ -1811,12 +1811,12 @@
       <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="69"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="28"/>
-      <c r="D24" s="74"/>
+      <c r="D24" s="68"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1825,12 +1825,12 @@
       <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="69"/>
+      <c r="A25" s="64"/>
       <c r="B25" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="28"/>
-      <c r="D25" s="75"/>
+      <c r="D25" s="67"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1839,7 +1839,7 @@
       <c r="J25" s="32"/>
     </row>
     <row r="26" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="70"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="21" t="s">
         <v>25</v>
       </c>
@@ -1853,7 +1853,7 @@
       <c r="J26" s="32"/>
     </row>
     <row r="27" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="68">
+      <c r="A27" s="63">
         <v>3</v>
       </c>
       <c r="B27" s="22" t="s">
@@ -1869,13 +1869,13 @@
       <c r="J27" s="32"/>
     </row>
     <row r="28" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="69"/>
+      <c r="A28" s="64"/>
       <c r="B28" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="73" t="s">
+      <c r="E28" s="66" t="s">
         <v>70</v>
       </c>
       <c r="F28" s="4"/>
@@ -1885,13 +1885,13 @@
       <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="69"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="31"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="74"/>
+      <c r="E29" s="68"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -1899,13 +1899,13 @@
       <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="69"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="31"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="75"/>
+      <c r="E30" s="67"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -1913,7 +1913,7 @@
       <c r="J30" s="32"/>
     </row>
     <row r="31" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="69"/>
+      <c r="A31" s="64"/>
       <c r="B31" s="17" t="s">
         <v>26</v>
       </c>
@@ -1927,13 +1927,13 @@
       <c r="J31" s="32"/>
     </row>
     <row r="32" spans="1:11" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="69"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="20" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="31"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="73" t="s">
+      <c r="E32" s="66" t="s">
         <v>75</v>
       </c>
       <c r="F32" s="4"/>
@@ -1943,13 +1943,13 @@
       <c r="J32" s="32"/>
     </row>
     <row r="33" spans="1:10" ht="20.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="69"/>
+      <c r="A33" s="64"/>
       <c r="B33" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C33" s="31"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="74"/>
+      <c r="E33" s="68"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -1957,13 +1957,13 @@
       <c r="J33" s="32"/>
     </row>
     <row r="34" spans="1:10" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="69"/>
+      <c r="A34" s="64"/>
       <c r="B34" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="31"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="75"/>
+      <c r="E34" s="67"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -1971,7 +1971,7 @@
       <c r="J34" s="32"/>
     </row>
     <row r="35" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="69"/>
+      <c r="A35" s="64"/>
       <c r="B35" s="17" t="s">
         <v>28</v>
       </c>
@@ -1985,13 +1985,13 @@
       <c r="J35" s="32"/>
     </row>
     <row r="36" spans="1:10" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="69"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="20" t="s">
         <v>29</v>
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="73" t="s">
+      <c r="E36" s="66" t="s">
         <v>76</v>
       </c>
       <c r="F36" s="4"/>
@@ -2001,13 +2001,13 @@
       <c r="J36" s="32"/>
     </row>
     <row r="37" spans="1:10" ht="20.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="69"/>
+      <c r="A37" s="64"/>
       <c r="B37" s="20" t="s">
         <v>30</v>
       </c>
       <c r="C37" s="31"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="74"/>
+      <c r="E37" s="68"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -2015,13 +2015,13 @@
       <c r="J37" s="32"/>
     </row>
     <row r="38" spans="1:10" ht="20.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="69"/>
+      <c r="A38" s="64"/>
       <c r="B38" s="20" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="31"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="74"/>
+      <c r="E38" s="68"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -2029,13 +2029,13 @@
       <c r="J38" s="32"/>
     </row>
     <row r="39" spans="1:10" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="69"/>
+      <c r="A39" s="64"/>
       <c r="B39" s="20" t="s">
         <v>32</v>
       </c>
       <c r="C39" s="31"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="75"/>
+      <c r="E39" s="67"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -2043,7 +2043,7 @@
       <c r="J39" s="32"/>
     </row>
     <row r="40" spans="1:10" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="70"/>
+      <c r="A40" s="65"/>
       <c r="B40" s="19" t="s">
         <v>33</v>
       </c>
@@ -2059,7 +2059,7 @@
       <c r="J40" s="32"/>
     </row>
     <row r="41" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="68">
+      <c r="A41" s="63">
         <v>4</v>
       </c>
       <c r="B41" s="22" t="s">
@@ -2075,14 +2075,14 @@
       <c r="J41" s="32"/>
     </row>
     <row r="42" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="69"/>
+      <c r="A42" s="64"/>
       <c r="B42" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C42" s="24"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
-      <c r="F42" s="73" t="s">
+      <c r="F42" s="66" t="s">
         <v>70</v>
       </c>
       <c r="G42" s="2"/>
@@ -2091,35 +2091,35 @@
       <c r="J42" s="32"/>
     </row>
     <row r="43" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="69"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C43" s="24"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-      <c r="F43" s="74"/>
+      <c r="F43" s="68"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="44"/>
       <c r="J43" s="32"/>
     </row>
     <row r="44" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="69"/>
+      <c r="A44" s="64"/>
       <c r="B44" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C44" s="24"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="75"/>
+      <c r="F44" s="67"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="44"/>
       <c r="J44" s="32"/>
     </row>
     <row r="45" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="69"/>
+      <c r="A45" s="64"/>
       <c r="B45" s="17" t="s">
         <v>34</v>
       </c>
@@ -2133,7 +2133,7 @@
       <c r="J45" s="32"/>
     </row>
     <row r="46" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="69"/>
+      <c r="A46" s="64"/>
       <c r="B46" s="20" t="s">
         <v>35</v>
       </c>
@@ -2149,7 +2149,7 @@
       <c r="J46" s="32"/>
     </row>
     <row r="47" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="69"/>
+      <c r="A47" s="64"/>
       <c r="B47" s="20" t="s">
         <v>36</v>
       </c>
@@ -2165,7 +2165,7 @@
       <c r="J47" s="32"/>
     </row>
     <row r="48" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="69"/>
+      <c r="A48" s="64"/>
       <c r="B48" s="20" t="s">
         <v>37</v>
       </c>
@@ -2181,7 +2181,7 @@
       <c r="J48" s="32"/>
     </row>
     <row r="49" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="70"/>
+      <c r="A49" s="65"/>
       <c r="B49" s="38" t="s">
         <v>38</v>
       </c>
@@ -2197,7 +2197,7 @@
       <c r="J49" s="32"/>
     </row>
     <row r="50" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="68">
+      <c r="A50" s="63">
         <v>5</v>
       </c>
       <c r="B50" s="22" t="s">
@@ -2213,7 +2213,7 @@
       <c r="J50" s="32"/>
     </row>
     <row r="51" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="69"/>
+      <c r="A51" s="64"/>
       <c r="B51" s="16" t="s">
         <v>17</v>
       </c>
@@ -2221,7 +2221,7 @@
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="73" t="s">
+      <c r="G51" s="66" t="s">
         <v>70</v>
       </c>
       <c r="H51" s="3"/>
@@ -2229,7 +2229,7 @@
       <c r="J51" s="32"/>
     </row>
     <row r="52" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="69"/>
+      <c r="A52" s="64"/>
       <c r="B52" s="16" t="s">
         <v>18</v>
       </c>
@@ -2237,13 +2237,13 @@
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="74"/>
+      <c r="G52" s="68"/>
       <c r="H52" s="3"/>
       <c r="I52" s="47"/>
       <c r="J52" s="32"/>
     </row>
     <row r="53" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="69"/>
+      <c r="A53" s="64"/>
       <c r="B53" s="16" t="s">
         <v>4</v>
       </c>
@@ -2251,13 +2251,13 @@
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="75"/>
+      <c r="G53" s="67"/>
       <c r="H53" s="3"/>
       <c r="I53" s="47"/>
       <c r="J53" s="32"/>
     </row>
     <row r="54" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="69"/>
+      <c r="A54" s="64"/>
       <c r="B54" s="17" t="s">
         <v>39</v>
       </c>
@@ -2271,7 +2271,7 @@
       <c r="J54" s="32"/>
     </row>
     <row r="55" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="69"/>
+      <c r="A55" s="64"/>
       <c r="B55" s="16" t="s">
         <v>40</v>
       </c>
@@ -2288,7 +2288,7 @@
       <c r="K55" s="7"/>
     </row>
     <row r="56" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="69"/>
+      <c r="A56" s="64"/>
       <c r="B56" s="16" t="s">
         <v>41</v>
       </c>
@@ -2305,7 +2305,7 @@
       <c r="K56" s="7"/>
     </row>
     <row r="57" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="69"/>
+      <c r="A57" s="64"/>
       <c r="B57" s="16" t="s">
         <v>42</v>
       </c>
@@ -2322,7 +2322,7 @@
       <c r="K57" s="18"/>
     </row>
     <row r="58" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="69"/>
+      <c r="A58" s="64"/>
       <c r="B58" s="17" t="s">
         <v>43</v>
       </c>
@@ -2336,7 +2336,7 @@
       <c r="J58" s="32"/>
     </row>
     <row r="59" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="69"/>
+      <c r="A59" s="64"/>
       <c r="B59" s="16" t="s">
         <v>44</v>
       </c>
@@ -2352,7 +2352,7 @@
       <c r="J59" s="32"/>
     </row>
     <row r="60" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="69"/>
+      <c r="A60" s="64"/>
       <c r="B60" s="16" t="s">
         <v>45</v>
       </c>
@@ -2368,7 +2368,7 @@
       <c r="J60" s="32"/>
     </row>
     <row r="61" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="69"/>
+      <c r="A61" s="64"/>
       <c r="B61" s="16" t="s">
         <v>46</v>
       </c>
@@ -2384,7 +2384,7 @@
       <c r="J61" s="32"/>
     </row>
     <row r="62" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="69"/>
+      <c r="A62" s="64"/>
       <c r="B62" s="17" t="s">
         <v>47</v>
       </c>
@@ -2398,7 +2398,7 @@
       <c r="J62" s="32"/>
     </row>
     <row r="63" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="69"/>
+      <c r="A63" s="64"/>
       <c r="B63" s="16" t="s">
         <v>48</v>
       </c>
@@ -2414,7 +2414,7 @@
       <c r="J63" s="32"/>
     </row>
     <row r="64" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="69"/>
+      <c r="A64" s="64"/>
       <c r="B64" s="17" t="s">
         <v>49</v>
       </c>
@@ -2428,7 +2428,7 @@
       <c r="J64" s="32"/>
     </row>
     <row r="65" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="69"/>
+      <c r="A65" s="64"/>
       <c r="B65" s="16" t="s">
         <v>50</v>
       </c>
@@ -2444,7 +2444,7 @@
       <c r="J65" s="32"/>
     </row>
     <row r="66" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="70"/>
+      <c r="A66" s="65"/>
       <c r="B66" s="19" t="s">
         <v>51</v>
       </c>
@@ -2460,7 +2460,7 @@
       <c r="J66" s="32"/>
     </row>
     <row r="67" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="68">
+      <c r="A67" s="63">
         <v>6</v>
       </c>
       <c r="B67" s="22" t="s">
@@ -2476,7 +2476,7 @@
       <c r="J67" s="32"/>
     </row>
     <row r="68" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="69"/>
+      <c r="A68" s="64"/>
       <c r="B68" s="16" t="s">
         <v>17</v>
       </c>
@@ -2485,14 +2485,14 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
-      <c r="H68" s="73" t="s">
+      <c r="H68" s="66" t="s">
         <v>70</v>
       </c>
       <c r="I68" s="50"/>
       <c r="J68" s="32"/>
     </row>
     <row r="69" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="69"/>
+      <c r="A69" s="64"/>
       <c r="B69" s="16" t="s">
         <v>18</v>
       </c>
@@ -2501,12 +2501,12 @@
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
-      <c r="H69" s="74"/>
+      <c r="H69" s="68"/>
       <c r="I69" s="50"/>
       <c r="J69" s="32"/>
     </row>
     <row r="70" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="69"/>
+      <c r="A70" s="64"/>
       <c r="B70" s="16" t="s">
         <v>4</v>
       </c>
@@ -2515,12 +2515,12 @@
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
-      <c r="H70" s="75"/>
+      <c r="H70" s="67"/>
       <c r="I70" s="50"/>
       <c r="J70" s="32"/>
     </row>
     <row r="71" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="69"/>
+      <c r="A71" s="64"/>
       <c r="B71" s="17" t="s">
         <v>52</v>
       </c>
@@ -2534,7 +2534,7 @@
       <c r="J71" s="32"/>
     </row>
     <row r="72" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="69"/>
+      <c r="A72" s="64"/>
       <c r="B72" s="16" t="s">
         <v>53</v>
       </c>
@@ -2550,7 +2550,7 @@
       <c r="J72" s="32"/>
     </row>
     <row r="73" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="69"/>
+      <c r="A73" s="64"/>
       <c r="B73" s="17" t="s">
         <v>54</v>
       </c>
@@ -2564,7 +2564,7 @@
       <c r="J73" s="32"/>
     </row>
     <row r="74" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="69"/>
+      <c r="A74" s="64"/>
       <c r="B74" s="16" t="s">
         <v>55</v>
       </c>
@@ -2573,14 +2573,14 @@
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
-      <c r="H74" s="73" t="s">
+      <c r="H74" s="66" t="s">
         <v>72</v>
       </c>
       <c r="I74" s="50"/>
       <c r="J74" s="32"/>
     </row>
     <row r="75" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="69"/>
+      <c r="A75" s="64"/>
       <c r="B75" s="16" t="s">
         <v>56</v>
       </c>
@@ -2589,12 +2589,12 @@
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
-      <c r="H75" s="75"/>
+      <c r="H75" s="67"/>
       <c r="I75" s="50"/>
       <c r="J75" s="32"/>
     </row>
     <row r="76" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="69"/>
+      <c r="A76" s="64"/>
       <c r="B76" s="16" t="s">
         <v>57</v>
       </c>
@@ -2610,7 +2610,7 @@
       <c r="J76" s="32"/>
     </row>
     <row r="77" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="69"/>
+      <c r="A77" s="64"/>
       <c r="B77" s="17" t="s">
         <v>58</v>
       </c>
@@ -2624,7 +2624,7 @@
       <c r="J77" s="32"/>
     </row>
     <row r="78" spans="1:10" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="69"/>
+      <c r="A78" s="64"/>
       <c r="B78" s="20" t="s">
         <v>59</v>
       </c>
@@ -2640,7 +2640,7 @@
       <c r="J78" s="32"/>
     </row>
     <row r="79" spans="1:10" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="69"/>
+      <c r="A79" s="64"/>
       <c r="B79" s="40" t="s">
         <v>60</v>
       </c>
@@ -2656,7 +2656,7 @@
       <c r="J79" s="32"/>
     </row>
     <row r="80" spans="1:10" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="70"/>
+      <c r="A80" s="65"/>
       <c r="B80" s="21" t="s">
         <v>61</v>
       </c>
@@ -2672,7 +2672,7 @@
       <c r="J80" s="32"/>
     </row>
     <row r="81" spans="1:10" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="68">
+      <c r="A81" s="63">
         <v>7</v>
       </c>
       <c r="B81" s="22" t="s">
@@ -2688,7 +2688,7 @@
       <c r="J81" s="32"/>
     </row>
     <row r="82" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="69"/>
+      <c r="A82" s="64"/>
       <c r="B82" s="16" t="s">
         <v>17</v>
       </c>
@@ -2698,13 +2698,13 @@
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
-      <c r="I82" s="76" t="s">
+      <c r="I82" s="60" t="s">
         <v>70</v>
       </c>
       <c r="J82" s="32"/>
     </row>
     <row r="83" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="69"/>
+      <c r="A83" s="64"/>
       <c r="B83" s="16" t="s">
         <v>63</v>
       </c>
@@ -2714,11 +2714,11 @@
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
-      <c r="I83" s="77"/>
+      <c r="I83" s="61"/>
       <c r="J83" s="32"/>
     </row>
     <row r="84" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="69"/>
+      <c r="A84" s="64"/>
       <c r="B84" s="16" t="s">
         <v>4</v>
       </c>
@@ -2728,11 +2728,11 @@
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
-      <c r="I84" s="78"/>
+      <c r="I84" s="62"/>
       <c r="J84" s="32"/>
     </row>
     <row r="85" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="69"/>
+      <c r="A85" s="64"/>
       <c r="B85" s="17" t="s">
         <v>64</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="J85" s="32"/>
     </row>
     <row r="86" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="69"/>
+      <c r="A86" s="64"/>
       <c r="B86" s="16" t="s">
         <v>65</v>
       </c>
@@ -2762,7 +2762,7 @@
       <c r="J86" s="32"/>
     </row>
     <row r="87" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="69"/>
+      <c r="A87" s="64"/>
       <c r="B87" s="17" t="s">
         <v>66</v>
       </c>
@@ -2776,7 +2776,7 @@
       <c r="J87" s="32"/>
     </row>
     <row r="88" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="69"/>
+      <c r="A88" s="64"/>
       <c r="B88" s="16" t="s">
         <v>67</v>
       </c>
@@ -2786,13 +2786,13 @@
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
-      <c r="I88" s="76" t="s">
+      <c r="I88" s="60" t="s">
         <v>77</v>
       </c>
       <c r="J88" s="32"/>
     </row>
     <row r="89" spans="1:10" ht="30.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="69"/>
+      <c r="A89" s="64"/>
       <c r="B89" s="20" t="s">
         <v>68</v>
       </c>
@@ -2802,11 +2802,11 @@
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
-      <c r="I89" s="77"/>
+      <c r="I89" s="61"/>
       <c r="J89" s="32"/>
     </row>
     <row r="90" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="70"/>
+      <c r="A90" s="65"/>
       <c r="B90" s="19" t="s">
         <v>69</v>
       </c>
@@ -2816,19 +2816,17 @@
       <c r="F90" s="11"/>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
-      <c r="I90" s="78"/>
+      <c r="I90" s="62"/>
       <c r="J90" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="I88:I90"/>
-    <mergeCell ref="A81:A90"/>
-    <mergeCell ref="A41:A49"/>
-    <mergeCell ref="A50:A66"/>
-    <mergeCell ref="A67:A80"/>
-    <mergeCell ref="H74:H75"/>
-    <mergeCell ref="H68:H70"/>
-    <mergeCell ref="I82:I84"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A3:A15"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="E28:E30"/>
     <mergeCell ref="F42:F44"/>
@@ -2838,12 +2836,14 @@
     <mergeCell ref="E36:E39"/>
     <mergeCell ref="E32:E34"/>
     <mergeCell ref="A27:A40"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A3:A15"/>
-    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="I88:I90"/>
+    <mergeCell ref="A81:A90"/>
+    <mergeCell ref="A41:A49"/>
+    <mergeCell ref="A50:A66"/>
+    <mergeCell ref="A67:A80"/>
+    <mergeCell ref="H74:H75"/>
+    <mergeCell ref="H68:H70"/>
+    <mergeCell ref="I82:I84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2851,20 +2851,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d40eec68-307d-43ee-b57a-d8f7027588ad" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d40eec68-307d-43ee-b57a-d8f7027588ad" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3069,6 +3069,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E92328C1-AC67-4560-BD67-F4A51B4BF64C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3819C419-123F-4A1E-A541-86931FAD9C2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3081,14 +3089,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="f6ea39e4-54d2-4e84-95b0-d4fb9253a142"/>
     <ds:schemaRef ds:uri="d40eec68-307d-43ee-b57a-d8f7027588ad"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E92328C1-AC67-4560-BD67-F4A51B4BF64C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>